<commit_message>
explain identifier resource; add to CSV templates
</commit_message>
<xml_diff>
--- a/docs/files/SubmissionTemplate.xlsx
+++ b/docs/files/SubmissionTemplate.xlsx
@@ -58,7 +58,7 @@
                 <xdr:col>5</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>9</xdr:rowOff>
+                <xdr:rowOff>8</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -107,7 +107,7 @@
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
                 <xdr:row>10</xdr:row>
-                <xdr:rowOff>4</xdr:rowOff>
+                <xdr:rowOff>3</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -143,7 +143,7 @@
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
                 <xdr:row>10</xdr:row>
-                <xdr:rowOff>13</xdr:rowOff>
+                <xdr:rowOff>12</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -192,7 +192,7 @@
                 <xdr:col>8</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
                 <xdr:row>10</xdr:row>
-                <xdr:rowOff>11</xdr:rowOff>
+                <xdr:rowOff>10</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -239,7 +239,7 @@
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>8</xdr:row>
-                <xdr:rowOff>10</xdr:rowOff>
+                <xdr:rowOff>9</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -291,7 +291,7 @@
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>15</xdr:row>
-                <xdr:rowOff>3</xdr:rowOff>
+                <xdr:rowOff>2</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -345,7 +345,7 @@
                 <xdr:col>11</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>17</xdr:row>
-                <xdr:rowOff>11</xdr:rowOff>
+                <xdr:rowOff>10</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -382,7 +382,7 @@
                 <xdr:col>12</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>13</xdr:rowOff>
+                <xdr:rowOff>12</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -419,7 +419,7 @@
                 <xdr:col>13</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>13</xdr:rowOff>
+                <xdr:rowOff>12</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -465,7 +465,7 @@
                 <xdr:col>14</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
                 <xdr:row>21</xdr:row>
-                <xdr:rowOff>5</xdr:rowOff>
+                <xdr:rowOff>4</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -513,7 +513,7 @@
                 <xdr:col>15</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
                 <xdr:row>8</xdr:row>
-                <xdr:rowOff>2</xdr:rowOff>
+                <xdr:rowOff>1</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -551,7 +551,7 @@
                 <xdr:col>16</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>11</xdr:row>
-                <xdr:rowOff>12</xdr:rowOff>
+                <xdr:rowOff>11</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -587,7 +587,7 @@
                 <xdr:col>17</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>13</xdr:rowOff>
+                <xdr:rowOff>12</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -624,7 +624,7 @@
                 <xdr:col>18</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>9</xdr:row>
-                <xdr:rowOff>1</xdr:rowOff>
+                <xdr:rowOff>0</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -661,7 +661,7 @@
                 <xdr:col>19</xdr:col>
                 <xdr:colOff>11</xdr:colOff>
                 <xdr:row>8</xdr:row>
-                <xdr:rowOff>3</xdr:rowOff>
+                <xdr:rowOff>2</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -695,9 +695,9 @@
               </xdr:from>
               <xdr:to>
                 <xdr:col>20</xdr:col>
-                <xdr:colOff>7</xdr:colOff>
+                <xdr:colOff>8</xdr:colOff>
                 <xdr:row>10</xdr:row>
-                <xdr:rowOff>4</xdr:rowOff>
+                <xdr:rowOff>3</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -741,10 +741,10 @@
                 <xdr:rowOff>29</xdr:rowOff>
               </xdr:from>
               <xdr:to>
-                <xdr:col>20</xdr:col>
-                <xdr:colOff>119</xdr:colOff>
+                <xdr:col>21</xdr:col>
+                <xdr:colOff>1</xdr:colOff>
                 <xdr:row>11</xdr:row>
-                <xdr:rowOff>4</xdr:rowOff>
+                <xdr:rowOff>3</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -752,7 +752,7 @@
         <mc:Fallback/>
       </mc:AlternateContent>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="R1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -774,7 +774,8 @@
           </rPr>
           <t xml:space="preserve">REQUIRED, CONDITIONALLY; MULTIPLE VALUES POSSIBLE
 At least one Institution must be linked to each Report.
-A local identifier used by the Agency to identify each institution. If it has already been provided through the administrative interface or EQAR secretariat, you may identify the Institution with a single local identifier as &lt;identifier&gt; instead of a &lt;deqar_id&gt; or a &lt;eter_id&gt;.</t>
+A local or other identifier used to identify the institution. If it has already been provided through the administrative interface or EQAR secretariat, you may identify the Institution with a single local identifier as &lt;identifier&gt; instead of a &lt;deqar_id&gt; or a &lt;eter_id&gt;.
+If you use a local identifier (associated to your agency) you only need this column; if you use another (global) identifier you must also include the following column, &lt;resource&gt;.</t>
         </r>
       </text>
       <mc:AlternateContent>
@@ -789,9 +790,9 @@
               </xdr:from>
               <xdr:to>
                 <xdr:col>21</xdr:col>
-                <xdr:colOff>108</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>3</xdr:rowOff>
+                <xdr:colOff>113</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>11</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -800,6 +801,53 @@
       </mc:AlternateContent>
     </comment>
     <comment ref="S1" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FFFF0000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+          </rPr>
+          <t xml:space="preserve">USE ONLY as alternative to DEQARINST ID and when identifier is not a local identifier of your agency.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+          </rPr>
+          <t xml:space="preserve">REQUIRED, CONDITIONALLY; MULTIPLE VALUES POSSIBLE
+At least one Institution must be linked to each Report.
+If the identifier you use is not a local identifier of your agency, you need to provide its corresponding resource tag. The value for this field can be consulted through the administrative interface.</t>
+        </r>
+      </text>
+      <mc:AlternateContent>
+        <mc:Choice Requires="v2">
+          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
+            <anchor moveWithCells="false" sizeWithCells="false">
+              <xdr:from>
+                <xdr:col>19</xdr:col>
+                <xdr:colOff>15</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>34</xdr:rowOff>
+              </xdr:from>
+              <xdr:to>
+                <xdr:col>22</xdr:col>
+                <xdr:colOff>108</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>2</xdr:rowOff>
+              </xdr:to>
+            </anchor>
+          </commentPr>
+        </mc:Choice>
+        <mc:Fallback/>
+      </mc:AlternateContent>
+    </comment>
+    <comment ref="T1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -819,16 +867,16 @@
           <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
-                <xdr:col>19</xdr:col>
+                <xdr:col>20</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>40</xdr:rowOff>
               </xdr:from>
               <xdr:to>
-                <xdr:col>23</xdr:col>
+                <xdr:col>24</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>8</xdr:row>
-                <xdr:rowOff>3</xdr:rowOff>
+                <xdr:rowOff>2</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -836,7 +884,7 @@
         <mc:Fallback/>
       </mc:AlternateContent>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -856,16 +904,16 @@
           <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
-                <xdr:col>20</xdr:col>
+                <xdr:col>21</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>40</xdr:rowOff>
               </xdr:from>
               <xdr:to>
-                <xdr:col>24</xdr:col>
+                <xdr:col>25</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>8</xdr:row>
-                <xdr:rowOff>3</xdr:rowOff>
+                <xdr:rowOff>2</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -873,7 +921,7 @@
         <mc:Fallback/>
       </mc:AlternateContent>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -892,16 +940,16 @@
           <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
-                <xdr:col>21</xdr:col>
+                <xdr:col>22</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>46</xdr:rowOff>
               </xdr:from>
               <xdr:to>
-                <xdr:col>25</xdr:col>
+                <xdr:col>26</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>13</xdr:rowOff>
+                <xdr:rowOff>12</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -909,7 +957,7 @@
         <mc:Fallback/>
       </mc:AlternateContent>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -928,16 +976,16 @@
           <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
-                <xdr:col>22</xdr:col>
+                <xdr:col>23</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>46</xdr:rowOff>
               </xdr:from>
               <xdr:to>
-                <xdr:col>26</xdr:col>
+                <xdr:col>27</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>13</xdr:rowOff>
+                <xdr:rowOff>12</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -945,7 +993,7 @@
         <mc:Fallback/>
       </mc:AlternateContent>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -965,16 +1013,16 @@
           <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
-                <xdr:col>23</xdr:col>
+                <xdr:col>24</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>46</xdr:rowOff>
               </xdr:from>
               <xdr:to>
-                <xdr:col>27</xdr:col>
+                <xdr:col>28</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>13</xdr:rowOff>
+                <xdr:rowOff>12</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -982,7 +1030,7 @@
         <mc:Fallback/>
       </mc:AlternateContent>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1003,16 +1051,16 @@
           <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
-                <xdr:col>24</xdr:col>
+                <xdr:col>25</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>46</xdr:rowOff>
               </xdr:from>
               <xdr:to>
-                <xdr:col>28</xdr:col>
+                <xdr:col>29</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>10</xdr:row>
-                <xdr:rowOff>4</xdr:rowOff>
+                <xdr:rowOff>3</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -1020,7 +1068,7 @@
         <mc:Fallback/>
       </mc:AlternateContent>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1040,16 +1088,16 @@
           <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
-                <xdr:col>25</xdr:col>
+                <xdr:col>26</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>46</xdr:rowOff>
               </xdr:from>
               <xdr:to>
-                <xdr:col>29</xdr:col>
+                <xdr:col>30</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>13</xdr:rowOff>
+                <xdr:rowOff>12</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -1057,7 +1105,7 @@
         <mc:Fallback/>
       </mc:AlternateContent>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1080,16 +1128,16 @@
           <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
-                <xdr:col>26</xdr:col>
+                <xdr:col>27</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>46</xdr:rowOff>
               </xdr:from>
               <xdr:to>
-                <xdr:col>30</xdr:col>
+                <xdr:col>31</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>13</xdr:row>
-                <xdr:rowOff>16</xdr:rowOff>
+                <xdr:rowOff>15</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -1097,7 +1145,7 @@
         <mc:Fallback/>
       </mc:AlternateContent>
     </comment>
-    <comment ref="AA1" authorId="1">
+    <comment ref="AB1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1116,16 +1164,16 @@
           <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="top">
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
-                <xdr:col>27</xdr:col>
+                <xdr:col>28</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>46</xdr:rowOff>
               </xdr:from>
               <xdr:to>
-                <xdr:col>31</xdr:col>
+                <xdr:col>32</xdr:col>
                 <xdr:colOff>15</xdr:colOff>
                 <xdr:row>13</xdr:row>
-                <xdr:rowOff>16</xdr:rowOff>
+                <xdr:rowOff>15</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -1138,7 +1186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="139">
   <si>
     <t xml:space="preserve">agency</t>
   </si>
@@ -1192,6 +1240,9 @@
   </si>
   <si>
     <t xml:space="preserve">institution[1].identifier[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">institution[1].resource[1]</t>
   </si>
   <si>
     <t xml:space="preserve">programme[1].identifier[1]</t>
@@ -1943,7 +1994,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA1048576"/>
+  <dimension ref="A1:AB1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1961,13 +2012,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="22" style="0" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="15.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="23" style="0" width="16.2"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="37.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="38.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2022,7 +2073,7 @@
       <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="3" t="s">
@@ -2046,8 +2097,11 @@
       <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3062,7 +3116,7 @@
   </sheetPr>
   <dimension ref="A1:AF996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3091,7 +3145,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="65" style="0" width="16.2"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3129,40 +3183,40 @@
         <v>14</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y1" s="10" t="s">
         <v>15</v>
@@ -3174,24 +3228,24 @@
         <v>17</v>
       </c>
       <c r="AB1" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="101.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="105.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F2" s="13" t="n">
         <v>43546</v>
@@ -3200,73 +3254,73 @@
         <v>45747</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="R2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="X2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="Y2" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Z2" s="12"/>
       <c r="AA2" s="14"/>
       <c r="AB2" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AC2" s="14"/>
       <c r="AD2" s="14"/>
       <c r="AE2" s="14"/>
       <c r="AF2" s="14"/>
     </row>
-    <row r="3" customFormat="false" ht="90.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="93.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>97</v>
@@ -3282,26 +3336,26 @@
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="O3" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
@@ -3313,7 +3367,7 @@
       <c r="W3" s="11"/>
       <c r="X3" s="12"/>
       <c r="Y3" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z3" s="12"/>
       <c r="AA3" s="14"/>
@@ -6320,7 +6374,7 @@
   </sheetPr>
   <dimension ref="A1:AP996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6348,10 +6402,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="34" style="11" width="16.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="11" width="34.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="43" style="11" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="65" style="0" width="16.2"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6389,22 +6442,22 @@
         <v>14</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S1" s="10" t="s">
         <v>15</v>
@@ -6413,157 +6466,157 @@
         <v>16</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AC1" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AD1" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AE1" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF1" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AG1" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AH1" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AI1" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AJ1" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AK1" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AL1" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AN1" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AO1" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AP1" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="79.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="82.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="13" t="n">
         <v>43538</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
       <c r="S2" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="U2" s="15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
       <c r="AA2" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AB2" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AD2" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE2" s="12"/>
       <c r="AF2" s="6"/>
       <c r="AH2" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="90.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="93.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>184</v>
@@ -6581,97 +6634,97 @@
         <v>45473</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
       <c r="S3" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="T3" s="12"/>
       <c r="U3" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="V3" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="X3" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Z3" s="0"/>
       <c r="AA3" s="12" t="n">
         <v>2</v>
       </c>
       <c r="AB3" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AC3" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AD3" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AE3" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AF3" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AG3" s="15"/>
       <c r="AH3" s="12" t="n">
         <v>1</v>
       </c>
       <c r="AI3" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ3" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AK3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AL3" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM3" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="AJ3" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="AK3" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="AL3" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="AM3" s="11" t="s">
-        <v>100</v>
       </c>
       <c r="AO3" s="11" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="68.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="70.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>181</v>
@@ -6686,68 +6739,68 @@
         <v>43280</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="T4" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U4" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V4" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="W4" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Y4" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Z4" s="0"/>
       <c r="AA4" s="12" t="n">
         <v>2</v>
       </c>
       <c r="AB4" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AC4" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AD4" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AF4" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AH4" s="11" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="101.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="105.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F5" s="16" t="n">
         <v>43999</v>
@@ -6756,72 +6809,72 @@
         <v>46203</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="T5" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="U5" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="V5" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="W5" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="X5" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Z5" s="12"/>
       <c r="AA5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB5" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC5" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD5" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AB5" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="AC5" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD5" s="12" t="s">
-        <v>88</v>
-      </c>
       <c r="AE5" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AH5" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AP5" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14772,7 +14825,7 @@
   </sheetPr>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -14798,7 +14851,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="25" style="0" width="16.2"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="37.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="38.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14839,48 +14892,48 @@
         <v>16</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="123.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="128.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F2" s="21" t="n">
         <v>41654</v>
@@ -14889,47 +14942,47 @@
         <v>43130</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O2" s="20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R2" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="S2" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="U2" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V2" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -14950,9 +15003,9 @@
   </sheetPr>
   <dimension ref="A1:BN999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -14983,10 +15036,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="23" width="16.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="23" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="59" style="23" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="65" style="0" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="65" style="0" width="16.2"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -15024,40 +15077,40 @@
         <v>14</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y1" s="10" t="s">
         <v>15</v>
@@ -15066,90 +15119,90 @@
         <v>16</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AD1" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE1" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AF1" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AG1" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AH1" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AI1" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AJ1" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AK1" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AL1" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AN1" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AO1" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AP1" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AQ1" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AR1" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AS1" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AT1" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AU1" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AV1" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AW1" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="90.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="105.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F2" s="13" t="n">
         <v>43546</v>
@@ -15158,56 +15211,56 @@
         <v>45747</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="R2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="X2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="Y2" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Z2" s="12"/>
       <c r="AA2" s="14"/>
@@ -15233,7 +15286,7 @@
       <c r="AU2" s="24"/>
       <c r="AV2" s="24"/>
       <c r="AW2" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AX2" s="24"/>
       <c r="AY2" s="25"/>
@@ -15245,12 +15298,12 @@
       <c r="BE2" s="25"/>
       <c r="BF2" s="25"/>
     </row>
-    <row r="3" customFormat="false" ht="90.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="93.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>97</v>
@@ -15266,26 +15319,26 @@
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="O3" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
@@ -15297,7 +15350,7 @@
       <c r="W3" s="11"/>
       <c r="X3" s="12"/>
       <c r="Y3" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Z3" s="12"/>
       <c r="AA3" s="14"/>
@@ -15333,47 +15386,47 @@
       <c r="BE3" s="25"/>
       <c r="BF3" s="25"/>
     </row>
-    <row r="4" customFormat="false" ht="68.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="82.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F4" s="13" t="n">
         <v>43538</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
@@ -15385,40 +15438,40 @@
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
       <c r="Y4" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Z4" s="11"/>
       <c r="AA4" s="12"/>
       <c r="AB4" s="12"/>
       <c r="AC4" s="12"/>
       <c r="AD4" s="15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AF4" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
       <c r="AI4" s="6"/>
       <c r="AJ4" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AK4" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AL4" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AM4" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AN4" s="12"/>
       <c r="AO4" s="6"/>
       <c r="AP4" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AQ4" s="11"/>
       <c r="AR4" s="11"/>
@@ -15443,12 +15496,12 @@
       <c r="BK4" s="25"/>
       <c r="BL4" s="25"/>
     </row>
-    <row r="5" customFormat="false" ht="90.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="93.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C5" s="12" t="n">
         <v>184</v>
@@ -15466,26 +15519,26 @@
         <v>45473</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
@@ -15497,63 +15550,63 @@
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
       <c r="Y5" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Z5" s="12"/>
       <c r="AA5" s="28"/>
       <c r="AB5" s="28"/>
       <c r="AC5" s="28"/>
       <c r="AD5" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AF5" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AG5" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AH5" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AI5" s="12"/>
       <c r="AJ5" s="12" t="n">
         <v>2</v>
       </c>
       <c r="AK5" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AL5" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AM5" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AN5" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AO5" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AP5" s="12" t="n">
         <v>1</v>
       </c>
       <c r="AQ5" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="AR5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AT5" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU5" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="AR5" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS5" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT5" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="AU5" s="11" t="s">
-        <v>100</v>
       </c>
       <c r="AV5" s="11" t="n">
         <v>1</v>
@@ -15575,12 +15628,12 @@
       <c r="BK5" s="25"/>
       <c r="BL5" s="25"/>
     </row>
-    <row r="6" customFormat="false" ht="68.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="70.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>181</v>
@@ -15596,17 +15649,17 @@
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
@@ -15622,40 +15675,40 @@
       <c r="X6" s="11"/>
       <c r="Y6" s="11"/>
       <c r="Z6" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AA6" s="11"/>
       <c r="AB6" s="11"/>
       <c r="AC6" s="11"/>
       <c r="AD6" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AE6" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AF6" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AG6" s="11"/>
       <c r="AH6" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AI6" s="12"/>
       <c r="AJ6" s="12" t="n">
         <v>2</v>
       </c>
       <c r="AK6" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AL6" s="17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AM6" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AN6" s="11"/>
       <c r="AO6" s="17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AP6" s="11" t="n">
         <v>1</v>
@@ -15683,21 +15736,21 @@
       <c r="BK6" s="25"/>
       <c r="BL6" s="25"/>
     </row>
-    <row r="7" customFormat="false" ht="101.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="105.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F7" s="16" t="n">
         <v>43999</v>
@@ -15706,35 +15759,35 @@
         <v>46203</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
@@ -15744,43 +15797,43 @@
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
       <c r="Z7" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
       <c r="AD7" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AE7" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AG7" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AH7" s="11"/>
       <c r="AI7" s="12"/>
       <c r="AJ7" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK7" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL7" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM7" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AK7" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="AL7" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AM7" s="12" t="s">
-        <v>88</v>
-      </c>
       <c r="AN7" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AO7" s="11"/>
       <c r="AP7" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AQ7" s="11"/>
       <c r="AR7" s="11"/>
@@ -15789,7 +15842,7 @@
       <c r="AU7" s="11"/>
       <c r="AV7" s="11"/>
       <c r="AW7" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AX7" s="24"/>
       <c r="AY7" s="24"/>
@@ -15808,21 +15861,21 @@
       <c r="BL7" s="24"/>
       <c r="BN7" s="30"/>
     </row>
-    <row r="8" customFormat="false" ht="90.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="100" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F8" s="21" t="n">
         <v>41654</v>
@@ -15831,17 +15884,17 @@
         <v>43130</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
@@ -15857,37 +15910,37 @@
       <c r="X8" s="22"/>
       <c r="Y8" s="22"/>
       <c r="Z8" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AA8" s="20" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AB8" s="20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AC8" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AD8" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AE8" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AF8" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AG8" s="20"/>
       <c r="AH8" s="20"/>
       <c r="AI8" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AJ8" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AK8" s="0"/>
       <c r="AW8" s="17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix: field name learning outcomes (ESCO)
</commit_message>
<xml_diff>
--- a/docs/files/SubmissionTemplate.xlsx
+++ b/docs/files/SubmissionTemplate.xlsx
@@ -1690,7 +1690,7 @@
     <t xml:space="preserve">programme[1].assessment_certification</t>
   </si>
   <si>
-    <t xml:space="preserve">programme[1].learning_outcome_esco[1]</t>
+    <t xml:space="preserve">programme[1].learning_outcome[1]</t>
   </si>
   <si>
     <t xml:space="preserve">programme[1].learning_outcome_description</t>
@@ -2757,7 +2757,7 @@
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3302,7 +3302,7 @@
   </sheetPr>
   <dimension ref="A1:AP5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3331,7 +3331,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="34.28"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3844,7 +3844,7 @@
   </sheetPr>
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -3867,7 +3867,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="27.61"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="40.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -4029,8 +4029,8 @@
   </sheetPr>
   <dimension ref="A1:AM3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AM2" activeCellId="0" sqref="AM2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC1" activeCellId="0" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4336,7 +4336,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="21.13"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="92" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="103.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
         <v>51</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="182.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="183.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
         <v>51</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="171.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="183.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
document Base64 file upload
</commit_message>
<xml_diff>
--- a/docs/files/SubmissionTemplate.xlsx
+++ b/docs/files/SubmissionTemplate.xlsx
@@ -340,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1">
+    <comment ref="O1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -356,7 +356,36 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1">
+    <comment ref="P1" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+          </rPr>
+          <t xml:space="preserve">ONE REQUIRED; MULTIPLE VALUES POSSIBLE
+Instead of providing a URL a file can also be submitted in-line as Base64-encoded data.
+&lt;file[n].file&gt; must be a Base64-encoded PDF document.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+          </rPr>
+          <t xml:space="preserve">ONE REQUIRED; MULTIPLE VALUES POSSIBLE
+If the file is provided inline as Base64-encoded data you must also provide a file name.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -372,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1">
+    <comment ref="S1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -388,7 +417,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -415,7 +444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1">
+    <comment ref="U1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -432,7 +461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1">
+    <comment ref="V1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -457,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1">
+    <comment ref="W1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -483,7 +512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="1">
+    <comment ref="X1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -509,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1">
+    <comment ref="Y1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -534,7 +563,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="2">
+    <comment ref="Z1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -549,7 +578,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="2">
+    <comment ref="AA1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -575,7 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="2">
+    <comment ref="AB1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -601,7 +630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="2">
+    <comment ref="AC1" authorId="2">
       <text>
         <r>
           <rPr>
@@ -626,7 +655,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="1">
+    <comment ref="AD1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -642,7 +671,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
+    <comment ref="AE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -658,7 +687,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
+    <comment ref="AF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -673,7 +702,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
+    <comment ref="AG1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -688,7 +717,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
+    <comment ref="AH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -704,7 +733,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -721,7 +750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="1">
+    <comment ref="AJ1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -750,7 +779,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -766,7 +795,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="1">
+    <comment ref="AL1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -797,7 +826,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="1">
+    <comment ref="AM1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -822,7 +851,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="1">
+    <comment ref="AN1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -852,7 +881,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="1">
+    <comment ref="AO1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -868,7 +897,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="1">
+    <comment ref="AP1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -886,7 +915,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="1">
+    <comment ref="AQ1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -904,7 +933,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="1">
+    <comment ref="AR1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -924,7 +953,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="192">
   <si>
     <t xml:space="preserve">agency</t>
   </si>
@@ -971,7 +1000,10 @@
     <t xml:space="preserve">file[1].original_location</t>
   </si>
   <si>
-    <t xml:space="preserve">file[1].content</t>
+    <t xml:space="preserve">file[1].file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file[1].file_name</t>
   </si>
   <si>
     <t xml:space="preserve">file[1].display_name</t>
@@ -1082,6 +1114,12 @@
     <t xml:space="preserve">file[3].original_location</t>
   </si>
   <si>
+    <t xml:space="preserve">file[3].file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file[3].file_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">file[3].display_name</t>
   </si>
   <si>
@@ -1175,6 +1213,16 @@
     <t xml:space="preserve">spa</t>
   </si>
   <si>
+    <t xml:space="preserve">JVBERi0xLjUKJbXtrvsKNCAwIG9iago8PCAvTGVuZ3RoIDUgMCBSCiAgIC9GaWx0ZXIgL0ZsYXRlRGVjb2RlCj4+CnN0cmVhbQp4nFWOwU7DMAyG734Kc2sOzZIuowmaEELiACeQInEADlHjboO0hSZj7O1JNwk2W7Jk//7tT6LIWcpctJJca1NfKmw6+AJxkMYVzpzAVYRbC5XhJodQR9d/a+bcaGN0jWbBlVTVvEbbwawtRSlQom3hpXhmUhcUAvqhpwu8Rxd2bh9xN/SeRvKsrGpdbFpkb/YBJipeLdB6KFy/z5a8uA0e6ZtG9NQMnjCtNxGZfT/bjq77DFmjn8Qn7UAhjxRLIYS8Pjf8zU5xTw8+BnJxOpjZO0KXsEk3aUvNB88MV69s+nJn4Ql+AUYtVRcKZW5kc3RyZWFtCmVuZG9iago1IDAgb2JqCiAgIDIzNAplbmRvYmoKMyAwIG9iago8PAogICAvRXh0R1N0YXRlIDw8CiAgICAgIC9hMCA8PCAvQ0EgMSAvY2EgMSA+PgogICA+PgogICAvRm9udCA8PAogICAgICAvZi0wLTAgNyAwIFIKICAgICAgL2YtMC0xIDggMCBSCiAgID4+Cj4+CmVuZG9iago5IDAgb2JqCjw8IC9UeXBlIC9PYmpTdG0KICAgL0xlbmd0aCAxMCAwIFIKICAgL04gMQogICAvRmlyc3QgNAogICAvRmlsdGVyIC9GbGF0ZURlY29kZQo+PgpzdHJlYW0KeJwzUzDgiuaK5QIABjgBXQplbmRzdHJlYW0KZW5kb2JqCjEwIDAgb2JqCiAgIDE2CmVuZG9iagoxMiAwIG9iago8PCAvTGVuZ3RoIDEzIDAgUgogICAvRmlsdGVyIC9GbGF0ZURlY29kZQogICAvTGVuZ3RoMSAxMjU1Ngo+PgpzdHJlYW0KeJztenl8U2W6//OePUvTJM3epElIkzTdF7qEFhpKN5YiUIEWKbSlLQVFAbFSFW5VEKmIC7Lzc0QdVpFQKqQgynjLNuNVcBQU0asjOjofe517LzozQpPfc05KLer44Q8/8/vnd07e867neZ/3+z7vs5wWCADIoQNocMxZ0LDww6+ezQYwvwRAzZjTtsSxadjoDwGsAgC9pmXh3AVTTuzzAtifAVA8OfeO9pa9TdO/Qgo43gytzQ1N2yv4bwFSErEtrxUb5MP4fKzPxHpi64IlS+9bq9RjvQPrD9xx15wGIFvPYv0a1jsWNCxdKKxTLgNIfQDrjoWLmxf2ahd1Yn0bAHMnUFCC+Vn2GHLLw5gQVKeEQMgIAYNJUIcAzmIS61imL2EZcx5zGnPZJTiCbwFMSzmClFjMM7NyNE6NF1MJszZ07U/sse/HhJiqqwdxFAE3AL8I51KSaYH1gows5dtlSxWryCMMW0HGU6V0JVMllMhXC6vkp6lT9Cn+tEJZo5jLtypWU4/Qj/CrFZupDfR6fotiN7WD/i2/RxErCLxcUJgFg3w6zykERk6NSipLYt0cx4NbqVTIGEIrKJrllCxQglxB84LKaLTwLPdIQKCZK3JKdqVDAeQRpTlm7SxTinmi+oqpqt/vt2AayMwTy5pLvzBBsbEIf1qjn6yqSu9bld43fkp7t0wuE+QhsiUQqyWEYlia4XiZIJMLYptcyzA0NoNSsWqZWjixKt3EpgjL1CdWCeofKuMntx8kBCh84xCSY5CIRFAmE6L0CBAKKQjq41JSs/f1m4Rek1RYJvRmZZLFdXWLoG5xnIzk4I+4ZMRF+omeTHifTCD6i+Hl58L7wnvPhTvYY1enMnvF9P0Y5o2ro6Sdr4xcZCzMWLBCIriJMtC+Udhs2WmnWRUVy+r0Km2sXhdQBnSCz0LGKw7Rp8hJ+lT8+8IHsvP2911fGr90KU5pTmmpmQLrTIzdYrAl+jmeNzhtVl5uMyjc/EbrTuth6wUr4zbEuq2sWa7kNSpvrM3LWryJ6bzXbPZ433XuqDOlpEy8UtV/eaL6u6q+d/v9Wr9fg0nrz6iD4uK+4j4sFfUXqfuwNStzTHugHFwIEUuxhGU4u0ej1qrj1Do1wyndw+ITPeAAm4ck2GRG3gMKvcpDYlQuixObWHwIJrkHYtT4gBS8iLooJUVMKckpyQ+SRXWwqK4ODEa89c4EkpOdn5efoyI8x3OuYaBRQw7xeD2uYbg/VPf5gjyt+to37JMbH781U3eAvyVrSvvoKafDfyGmPxG7Imncvgd2scTFVNw+dfId455/4URdXkXhU+mTrGrcKY5QpCTsuaf8oYOd5BJIZ2U1PkZKu+ML4Pmm5SyKLaF8QJsZdo+zsUTCqqiqv0iSToQnKzMuR+Na3d0tHjqkQUFB5CLdx74BCrDBvYHsfFWFarpqJ7M7nnULOirWpgbBZuPj5JTNqGDT49LVPo3WYld4LeYE+yrn4ugUVX24GzjP5cuAO4A/jV8TBd9issrkQIhJ4QGZFR9gpjwgjxc8BNFMSXnwwQehTmvIyc7LHS7ipAfEUoM85qoIIpg7XJvz3dPbl23fcd+ju0lndebIfc8Xv3TXwfD333xMZn954cwf/v3s76n84QnjKdv3o9bPqSFp3/+FTEdECiMfME5mIijBhEryyUDOJmGDerPht8wuYYd6tyEknBYuMJ+rvtIpRwiczcQrbVqFmTeb9ZQ31hIv8+rNlvgQkR10Lq77YYlVonBFpUxaXSoYGY8iTobL0lAewhuxxMZgSa5TeoCo8SEYOA+hVZy4XmnFeOGSE7W5wyXB0OsMOVqUFMqJq0V54alPVmZOOPLbDRteOE8SroX/9lH4GtH+mVtCYndsmPXMta69l+mL4a/DV8L94ZdJyjWiIgFUW7AC978Pz6cZLDArkHWYO8VRDKfjvLo2bgnP6pSUzqS2sTxwJoXcwlssoPTJLFaSbvKZwRxvDRHu4BCJuTxktUW4YI3fT8TzBHWkLi5HPwpFHUVe49JIq0B5VxGskRV7J+xpvTwp9bAtc3nAN64gLb6b7GQyNs2a8pvpz/dPpl5oLGqKMZTkLprX/zYyi3z3oQyHUIZZkMHwQDxamlv4ZJlcISpg1ItuDsxyRZNz6QPRXehFXdsbleaq4v4vogJNu2hNjt7V94esluGnTrHHwrb+FdQD1747i2fkDNJ/WjojxhAe4SMgmt70FIiaLCojM0s8EWfOnJFOBA1TIpeYCmQtFgqhCD4KFCRnErlaEa+0enMq1fNk89W8X9AqZXR8Np8os6mVtsIUKt1XeLiQKsxOdmvVPCtYvcOMCGhnwGW02XmvLV1B2XIVRXxRkVXH+5J3JVpGxfus42K9BeaRo14lG8EJPWQDDMjZFUnSLvf3DspacR/uhAaNSh3qtPS+9D6CucYYPWFJefn6YUDMbpIX6wRTQrwTDA6dk6A85VNOsNiMTqJ34gOu66+BU0fqEg2iwhqJIhRLUGPpSV5+9Bjifrqub7FOPJz5evE4ej1eMfPkDs/LjyOqxRNn125wtmYvaMyqJt2j9MqH73u80Cnfxf7thWNt9xjdygRNcqqnLtkgy3/rgfXHjmzsfHtG6tgdT+mtnCrGmjGX3CGkmtJmVk9Irj65tbJyU/9G6zCaXqnkSlyByvmvPLr+xThyWdRzWgB2O5OBPoEjsLyC2SOj1spIOT9WsYruFFbKf0/10if5M8JJ+RmFooWfLzTL5yna+HahTd6uWMl3KuTiWKqCvheWsvT0JEMSnkOmkBQyT5AnGG6o+eck8y8fMP9b0fr3ovXvReO/FY3/3OVDjP/g7yemvw6NdUDJ+rSIKfi06GGwq9Qp+BviCzwWiBN9AZ5jWHHgoD/wWEAl+gMKJS5belX0I/DdZb0mFp0ByReQCugr9A62oHWvW7RoERqjeConXjTuCjQZF9469/t3PuwOnzl68Y9Hw39gMq510xOu9dAVV8/RI6/9OwKK508fHkt/ifIuasnfB+7s1D9q2mmiec7IFWgrtTXaufy99L38Gt0m2Mhu0m80bDTugl0GdSWM11cYz+iZUvYkS61id8AOspPdZWQTk1iT3mggwOmViliboBKVqiEeAWWB7DfqTfuVTxhQt77rFNFEOK9UXTbdAGRU7BHibHOGqbioqAitO0HoAlq9HgyGBVqj0cQSsgClwrQqPUWERswEzBGFrMxFpA6FO4ejKZ5CK+zx5oqGOS9/FMlHZGjaecrzcGPJto5tHl9CRrI6O0PNjlKFl7xJ7ITJmBt+Kvz1y+GWbk54MYZzmoRnEpmJ1zbRD4lYlUQu0IeY8ZAOGSQ98ESBbBO7QbtZt0m/KZlLSnR785zlzorECu+0xOnelsS5nnZle0y7qs21JHGJe4lnR8Ku1DgaXQw2jUmPA4s+3mg16dN06UmxinmCx53nptzDYuRMSpzppNUWxzO29C0pigxeplJTPGQ4Myx2k8HkNY5K8vDeJEuWyu5VjwJvujkzq2vQL+q70u8X1Ue/X40l0THyZ4jKwu8XVYmoSUQ9skjSHBNIGuXRuy0ep8ruBJmHdxI6FXURm4wlmxbb4nUmJ3HEDnOCc5gqRvDKncTjlslJGuMEzoePBI3VScwGa1S7oGeE+kV6RA3dgLETbQZ6SJKR93oyRJcIVYioXniXZ8AKGg12InpROmnLyDeCu3RX06aR3rufWD16yYc9/3P7GGoP6xm1uWVeWdLEe98omffBx9+c4slhMmlG5vTpt5Ulokc5LHnsg5teXTujdWR2xcRAebI5zpaRWvbME2c/eI76R9Rfop5mKkADtwQ8XtoTk09XMIxKUFMqmUam9AqiedTIBUscEf0cMGvjQqQMzeLyIWZRdKOqinv7e0VwiSZqFAdMosGoTyfictDH2qt/8XbWZFPHqx99upvJ6MnbStGv0dT+xf2bIGqvSeFATJUXsPKfM8ggR8tleFLQ1/PxNJgF2RAnrre/qPe6G1dUXNUXdeVEu7fiMF5M8tXz7LE3Jb/QihMY2XfACFWBFN7GyW00idX5DTGcVm5G+qoYjc+o5bWxKruKUl3TmU3ma9HjKHrWdf5eyYEenAz9x+K+d3FCbX7ekDXizDi/Kzcn9xVXcbcm0Wg1K6Y4urq71q9nS4bPpKgXKTL15bXXmuhta3dJvmZH5DP6Y9Q1RtQ2swIjQrrTOkoWJ+jMcWZdEncvfYHnBWBVcuBi5Cz6YybeZFIYYtLlPqXCYiE+g9lseec6IoM+p+a6nSwu8muu+yhEozNK1i1XdCbzJX8cpU7jJgWWzIdfLXV376Fcw+eu+7w6jexnMvr9U4bX75rxfyjV1XPPjky+dfOU1dT7FhFLBfpVf0FViXsSSC8hJzBQmwutVCs9l1vFPMruhF2UUAGVVBkzjn2EWc2eYk6zwtiku5N4QXIfJVhRe4UiC7sxAHEwIfLwYZpeoKUIxWI5kMBxoiojLCeGgSxFczRwLCMXcKPo/dQRIkrKioNkP2dGZYmm55NP+gdNjmRxJCnU+nk0FOqJl6v4aJYiWiE35dPSNAOiiWF/RJxi6P2iTr5O90ZjFqXM8uoU/KF9wVCnblGcFDiSSySBpJwI33E8fA8alU1069VziBCFPven9Fn0uS0QDzsDGTvNZJNpl7DHRI8TNFt1NK3jbBY+xqZTxPPx8Ua1V0toL6Wx2OReo9lqCxEeve1lQze3z+//wePGgjrqdg/Ho+FW6jEoU8WpPUSriVXzZqyxQDvFAJtGofFArBYfMhN63gzhnGQgfIsGcJIbJPlAGLy5RHnmJU88WwrfXMOoqCt+/jPjfvXi5S+Ny3z06YUPm/cn/PXoO98T7btWZmLwwpyHdy14bvul1fe+d4LkfEEsZASiCcbIN5SMnYESPuUVlNzjKhIixQE3Y/AbaU4l11jEbSWcD/QqfSxtpyn6mijWeP6W/ez5y4gewD51/2XpxIunThLtAZ8MZRqP4K5De/d69FkxCTr7GO/yGU89xc4Iv7euv6wgTkHQWRIenEudWCfpBilOwHjPANWBVIzABSNvFLyMN+4e/h5BiIuh4jCS1Ng4Xq+Ux/jkFhPR+8BgNpp+FCAUSQGCKCditHc9OEAG8/LzbogNRGW4ojuQM/2hr6rTehKyVi081M2+0X9pstP/Qu2zYkzQll+z5Xz/abjOH+dGHe2BlYFCXuBVXKxRMKqMsV7Bq/LGVpqnKeYqlC633GJzmeUUY3Q7bUZbDIeaO97qpuPkSQiwxqcLEdJl8aFQkQDGn+lunwfM3qQQibkhylFfQYM5oOjQfUOoowYyeqIGNPvAioxDgp6BdQ1ZYVdgeO2ijompiUXPN78/Mfno7VXzNx+2+Ba27ETlv+mWxJHFieXTqrfdurY/n/ry9klrd/Q/RR1dkD3+2bfFlVPQFp7KuFE3qmAYLAmk7hZ2GqkkwWHVqDibno/lVDarYpiK8posifJ0dbrTNyzW7Epc5TxWN7iYywNbIoXgGv/A5w+rIR5Yi4fxQDwGpqwBH8Ss8gBt5AZicDEewIg0L3cglhONcQ4ZWLdWo47qTq/GRZ3c6S4/crTMjc9w+v68wG33HwofXrKlfUpmYXf7H9/pmHngaNOWB6bvoA+sHZtUFP4KY9TnN8zOTRjb/9F1XfopagoFuOCAXCgOcjkHgCsO0jkkqMwIxpyHAyDXaA9Qgt8vxmXxxCiLfqdK+Oq7f3wY3kjavwh/Fw5fJu1MRngVaWf7r/Z/SJ4O30m5Rfr78dEBF9GmegJxJHnge0gTmBm2yTmneeB8DWy3aEHz8TTtP3fu4kWQ7BO+z/wdbbIcdNAQyJ2nnKdtV96nZSp1NbpW3X06hhcSNGq1nKhiEwhQcoHitEpGptNlMRZDrMwNZr0hRBQHnetXD8wlnZJ+UaJEQ4qHOvpxitRlZdbFObMld8epcQEC79Q40T/aT63v/ev5j8PZp+iOpSV3h5eQNY/sZI99dPqlSP86pmeEPUwvflLk9dPIe3wh+zliOQ799tq8vOGV5c6pla2yud75o+aWLB152nyyTGFOMfuTRhbQBap8Jyf49XJvSbmiQlMDU+kaZ4vhdMxp1QXdBf2F0SqFHDWofJqcCcuJPC09I9UhpykhF43YkwctrnEU5l1pvkLMXomjK8aVj8FSQDNOJmfT0m3pBdlsrifbE1twjDyB5r0Yn7F89sqMvo9Qbfsz+jK0/o/SP9IiCv3vav3oTfT2qd8tEn0oo38Vqz4uOe5oYeoAJZCSNLE2F2iPRp2f53QYDRodDMSdAwEoiI5Ifg6tIlG1jS1OB8+JqtGZnZhv5BgX82n12MU7p41etbF/459euXSFbCVNb74e/mb3nFkMnfv8tPs3E3ZDy0ome93KWFW+a/Er4VfD/xVecealF4+TOTtIwr0lM8JbLtBH54T/d2XjXFL4b9dqCHuOaEn55XD3nvB/Xw4fmz1GYYq5e3bXmlMks616V3hczihTmu+/jn9JZB8fC//p+z1n5tXOmLRGlM0OlH1RthRoGZtqKTJCIGaKiHHWdHYu284t5VexPfQZ+iJKLcsJAi+jqRXUM+hE0ZRfK5MxLNpt9BRQYws8y2C4KhNYNHVylFmak/OcnLPEyCi5DxRmZUyXs7GHGGBQWRdh2CpZ9SJU2JKCE4FHhwGjx98xYhhZxy5TH1cLRUKRGExiJLkYdbn4pdhFeI2rYx9564twCznwRbhr4z722LW95FT4rv5GytoZvlM6O5/hIrsxIhD92eyABWMIOhk4XvJnWdLEiN7sD59xin74JFnVp5Z8Wb3ky352Di/GebF/3cWoPSgNz0Jf9j2IQy9ZKWggTo8EmQmxcUfJNhwgI9sCMsGs0//NWXz/gOvwLkrdkA+e6LVq1F4PnZNAjAlEj+qMrvhNevnk7HXtW0Z7Mn2zCo+EZ5G8tReIkzj/+gwxfHd387Iri8Lvf7k+/DFEuaClz0ZKYKiJmCeAGltU8G8QIdWkgSwly8nT1EnqksPjyHSMcLzkHBaJiH9LgefIFFKP/csG+uOw3z/Y/88vgnNcIlvINvIs3s8N3CfxPk1EQ8mA8KM3EgZL5n9C0zakHP+TXtkNNcuPuPnphXKHeyJ+eVRjSQ+x+LQiKgbcfw5VACA+MahHNaBFmTchdv//+snFHgc16oQktgMsaBftAJEPMF0U8/DUyBfsKVCHF0T+my7EwT1iosLFRXAcHoetaK042IXlJJgFm+AMmQ89ZCZ0w3mSAOmobxgIwQR4k0Qi56AFXsTxS+ANWI82VonvLMA9mwBriTtyH9YDWG6EFZHnIREK4BE4Bn6kuhb6IrsjB7F3CkyFPbAX3/8DcVEHmLjIy5HLKIOTkeYK7DkXmRDZjzudCiUwCVtXwGvETV+MtOLOFyJ32+A3sB1+B1+Th0h3pDXSFjkb+RRlx4QyU433MtJNPqX3M49EtkX+EgkjEkmQjLPWwzp4Aenvx/s4AVJGbidLyDqyngpQD1HdzErWGO5HHHxQgXcl3AWPIgI90Av/A/8g31AmWk0voU9EciP/i1I4HlcprqQZ2vBehfdaXNNRwpFMMoZMwlP6DFlP/kglU1OpGupeain1BT2Rnkm3039k7ma62DXsJk4R/jZyNHIq8h7KuA1ug8WwHFf3BpyFK/A9Qc+eWImbFJISMgvvDrKV6iHbSQ81iRwnZ6k95D/JZ+QbcpViKSWlp1KoJdQ6ai/1BvUWPY9eT2+m/5P+lhnFUux29nPOzX8YbgyvDr8Vwcgq8nc8XQI4cWdKYCLMhgZc7UIYjlpoLezDez/uWi+cgDPS/RmxQh/8HVEANFkWkk2q8J5IbiEtZB7qlCN4vybx8h2FG0HJKA1lpKxUNdVILaA6qPeoDjqeTqbH0TPo/Xifps/TV+mrDMvEMXrpC/kaZgGzBe8dzC6mi3mb9bOj2InsNLaDXc2uoeew59jz3HJuLdfFfcP9lU/iJ/B38Wtwd86gzP7uhmPAkETkPhvuhDmklDTCBtyN7aQBOlG6msijyONCSIrU0cvpCioTpeE1uB+ldQssg9X0TNgeeZ/eAxdQUu5AWh2wkykBG7sRd+chyEQp+uFeh7v+HLyE52Iv4gSQEp4qnTsn+xp4A75kX5LX4050DXM67Ak2a7zFbBI/SMWhCxyjVMhlAo8mmKYIpJa5yusdQU99kPG4KivTxLqrARsahjTUBx3YVH7jmKCjXhrmuHFkAEe2/GhkIDoyMDiSqB1FUJSW6ihzOYL/UepyhMiMyTVYfrzUVesI9knlKqn8pFSOwbLTiS84ykytpY4gqXeUBcvbWjvL6kuRXE8AIZCnpYqKJQAKkXAQxjQsazVhJo4oC1pcpWVBs6tU6qPdZQ1NwUmTa8pK453OWmzDpik1OEda6jyRT3hM2eRqeiwUgMZ6sdQwsyZIN9QGqXqRliYlaHSVBo33fW76oXq9VLZmSGeQcpc3NHeWIwSPVUar9WKtYQ3Wxlc7kCy1srYmSFYOMCHyOL80ym6zq0xsqp/vCMpcJa7Wzvn1CC5MqemyBCxlrobS2iBMqukyB8xSJS21x7S80Imr70kbnTZazAudpuXR/M8PR9vfOa6QxvV+gvn4KYMAEHEm11jkM+iYI03iQmYLxEdzAXTOKcBheNUSXOY85GdMkEKZod1B1j22IdhRfZ2N1tIoc/XzS7tkZou4hvqSWhxf36kegdPgeLXL0fkt4Ba6+r6+saVhoIVzq78FsShu9KCsYP/1cpsEjDidydUq7m9b2UDdZSob0oB1ERqR56AumD1+Uo0z6KjFhhCkpI4PgWxSzQFC1taGSGRlCEptPeg70LNnYXeqKGrzSnF+rKSlYkOyE0vpqY5yJFwuyoqj09E5tqnTUe5oRWFi3FKOHc2dtRmIYHUN4gS34oyB2vjBYnNt7QikkyHSYSQ6nbVIYf4AhfkSBSTQj4MyU8fjMj2TaibXBDtK44OB0lrcBRTf45Nqgsdx42prcVTWIKeYL5tnGuA5G3nOSsZCTpRKNdJAErWdndGayxk83tkZ3ymesWg9RODHDYGBhhBIBBDREOmYJHV1uJzxEuZOlxPZqhUxHY4ifV2iQpD7ywjnDUU4H7nNkxAu+JUQ9t8MwiNuCuHCn0e4CHkuFBEe+a9DeNQNCBf/MsKBoQiPRm4DEsIlvxLCY24G4dKbQrjs5xEuR57LRIQr/nUIV96A8NhfRnjcUITHI7fjJIQn/EoIV90MwhNvCuFbfh7hScjzLSLCk/91CE+5AeHqX0b41qEIT0Vub5UQnvYrITz9ZhCuuSmEa38e4RnIc62I8G2DCAfigzAU4Y4fAQq/OuQzb4C87pchnzUU8tnI/iwJ8vpfCfKGm4G88aYgn/PzkDchz3NEyJv/H0LeMgTy618d3u45smB2bNG3oIl+8phd9YSUf/xJ+vm/N1/zKp4S/gHi9wsy8AY+OV/YB6Ak2N+neOon3y/srBZK+MfBzdwNleQUrKb8GITcDQWYCjGtwHofpjNYnoIxuJYB0GMqofbAahwv9luxrwPbFJgKsW4U3+P2wArM28R2bNvPToP9gh0+xXoH1j/D90sHeMBYhcJmehOmS9HEdAOwLyL3MzG9iulrAKEDxP+hBQUuXnkaIOZWTEEAVSWmawDqJABNKqY3AbRIM64JQId9ul2YvkS2nwEw4pymREwPSB+HRDTsGDvK4Hbgpe83apgLwH+peBIYICjqKeQIsKQHZqeQ18lRGIVBpg/DKS2+2JzyOnkVA9AbW47BiBta4HVyGKpgJORjHH99EJ4GuEVqiR9o6cGYfeQNhI78iDRgkIpMNaWEyKGotEb//XgspmJMuSniP3WNNkEH2QFPYnoOEw3zyGPQjmk1ps2YmMHSbkw95LEuRggcIe1gIeMCCsZ+q85sN8kV9ndChOt+1v6B6bOjxAwx8Ckxd8WAbLScPEd+A01gJ78FN7kPKiGJbDnou8Nej127YSGmDky09CRkd1dCtv01kooCRvAdDyQw5JD9z1lp9s+zQhTpsr/hDTGY/S4Ba4FY+3Hbs/bXbXPtr2HaG+3a4wuJ7+y23WFflxAiW7rsT4t/y+qyPxXN7rHhq4fsC3wb7E1ZUv+EDSFqb5fdj/3TAgp7XoHTnmu7bM/whgSC9TTbBHty1n/YE23SMAcSdQc0dqttnX0EdiXYyrwjMB0le8hWSCZbu9zj7EewiMs9ONZXsCFE7j9YmZTlDpH7AnmVSRt8lV63b4Ld7Sv3erE87TS/gr+NH81n8ykY63t4Jx/P6wStoBZUglKQC4LAh8hLXcV27ijZC8UIy96DAiewIfIyNjJHyT6pcd9hgREoAQRdKPJJtyisuhDZ260WS1g4xEklLkT2HYw27QvYGbHESB1qSnxSUS1AEYGCcRgiPR7iYKWhrdhUrB2l8ZeX/rNH/Q3PlH9+mYgtuAFVVXCPrRYjJCxEbLWDnb/wYvRacg8+mkuk/ws42LZwfosU8bnKmjHVBx9rwwi8o9HhODB/4UA466lvnNMq5g3NwYWu5tLgfFep40Bby890t4jdba7SA9BSdmvNgZZAc2lXW6BNCnYPNpYsrrthrtWDcy0u+RliJSKxxeJcjXU/010ndjeKc9WJc9WJczUGGqW5xHWWzasuuXsJSicaHDQqSdXBsZNn1AQdDbWlIbJDtEL3APxfV/42FgplbmRzdHJlYW0KZW5kb2JqCjEzIDAgb2JqCiAgIDgwMDIKZW5kb2JqCjE0IDAgb2JqCjw8IC9MZW5ndGggMTUgMCBSCiAgIC9GaWx0ZXIgL0ZsYXRlRGVjb2RlCj4+CnN0cmVhbQp4nF2SzW6DMAzH73mKHLtDxTfpJIQ0dRcO+9DYHgASp0MaIQr0wNvPjqtO2gH8i/O3Y8dJzt1z56ZNJu9h0T1s0k7OBFiXa9AgR7hMTmS5NJPebqv41/PgRYLB/b5uMHfOLqJpZPKBm+sWdnl4MssID0JKmbwFA2FyF3n4Ovfs6q/e/8AMbpOpaFtpwGK6l8G/DjPIJAYfO4P707YfMexP8bl7kHlcZ1ySXgysftAQBncB0aRpKxtrWwHO/NsrUg4Zrf4egmgqhdI0RSOauoqMBlkza+Q8jYwG/SX7S2LLbImBGUifsT5DLh8jo0EN+2vyKz5X0bmKNYo0qmAuiHPmnGJZU8c8NXNNGq5ZUc2K/Yr8NeepYx6uWcWaT+w/ERtmQxruUVGPijWKNDn3lVNfFWsq0pTMZbyTkfOMyMUQGQ3Gcs1oaBC3G6eR0Nu5z1pfQ8AxxwcW50uTnRzc36BfPEXF7xdzDLT6CmVuZHN0cmVhbQplbmRvYmoKMTUgMCBvYmoKICAgMzYxCmVuZG9iagoxNiAwIG9iago8PCAvVHlwZSAvRm9udERlc2NyaXB0b3IKICAgL0ZvbnROYW1lIC9GT1BSTE0rSGVsdmV0aWNhCiAgIC9Gb250RmFtaWx5IChIZWx2ZXRpY2EpCiAgIC9GbGFncyAzMgogICAvRm9udEJCb3ggWyAtOTUwIC00ODAgMTQ0NSAxMTIxIF0KICAgL0l0YWxpY0FuZ2xlIDAKICAgL0FzY2VudCA3NzAKICAgL0Rlc2NlbnQgLTIyOQogICAvQ2FwSGVpZ2h0IDExMjEKICAgL1N0ZW1WIDgwCiAgIC9TdGVtSCA4MAogICAvRm9udEZpbGUyIDEyIDAgUgo+PgplbmRvYmoKNyAwIG9iago8PCAvVHlwZSAvRm9udAogICAvU3VidHlwZSAvVHJ1ZVR5cGUKICAgL0Jhc2VGb250IC9GT1BSTE0rSGVsdmV0aWNhCiAgIC9GaXJzdENoYXIgMzIKICAgL0xhc3RDaGFyIDEyMQogICAvRm9udERlc2NyaXB0b3IgMTYgMCBSCiAgIC9FbmNvZGluZyAvV2luQW5zaUVuY29kaW5nCiAgIC9XaWR0aHMgWyAyNzcuODMyMDMxIDI3Ny44MzIwMzEgMCAwIDAgMCAwIDAgMCAzMzMuMDA3ODEyIDAgMCAwIDAgMjc3LjgzMjAzMSAwIDAgMCAwIDAgMCAwIDAgMCAwIDAgMjc3LjgzMjAzMSAwIDAgMCAwIDAgMTAxNS4xMzY3MTkgMCAwIDAgMCAwIDAgMCAwIDI3Ny44MzIwMzEgMCAwIDAgMCAwIDAgNjY2Ljk5MjE4OCAwIDAgMCAwIDAgMCA5NDMuODQ3NjU2IDAgMCAwIDAgMCAwIDAgMCAwIDU1Ni4xNTIzNDQgMCA1MDAgNTU2LjE1MjM0NCA1NTYuMTUyMzQ0IDI3Ny44MzIwMzEgMCA1NTYuMTUyMzQ0IDIyMi4xNjc5NjkgMCA1MDAgMjIyLjE2Nzk2OSA4MzMuMDA3ODEyIDU1Ni4xNTIzNDQgNTU2LjE1MjM0NCA1NTYuMTUyMzQ0IDAgMzMzLjAwNzgxMiA1MDAgMjc3LjgzMjAzMSA1NTYuMTUyMzQ0IDUwMCA3MjIuMTY3OTY5IDUwMCA1MDAgXQogICAgL1RvVW5pY29kZSAxNCAwIFIKPj4KZW5kb2JqCjE3IDAgb2JqCjw8IC9MZW5ndGggMTggMCBSCiAgIC9GaWx0ZXIgL0ZsYXRlRGVjb2RlCiAgIC9MZW5ndGgxIDU0MTIKPj4Kc3RyZWFtCnicxVh7cFNlFj/nPpJbWta0gqQt6b3xkr7SCkXBliJNQ1JaWqC0wCZIIWmb0tZWu1izggObUXAlVBYXYRVclX24QkVu0w7elgUqg6POri7qyPqaVdbXzo6M+2JHRXv33JtSW6Yy/YNx882533l95zvf7zs36SkgACRABFiwNIQ7pUeuL30XAAUAtqupY317zQuHswC4hwESd61v29jk7VldTiseI2prDgUbDywyXwCwzCB5bjMpJl1vTiN5Dckzmts77zZXgpvkCMlC2x0NQZrfIvkBmpPag3d3COGkzSRTfJA6NoQ6Tqf8KEpyH+15OzD6Wu4Mf5yyM8NCFWqdKggzVeCIBIsKcIZIl4ln3yOeZjPNLM0J78EArQJY5RygSDzNswpuTLYnZxG5uZ3q13/lj3+1UOWWXOwF4AfBQvtk8xFI42aCCKC9TfSOPg+t1D7hXwTLULv2T7aYIvbrxAyVzIdBeBD2wxEwwdPEZ8NaeARexlboxzXQB2cxA24gbDlQoQr+iJr2GjTBb8i/E07BHuiBJFrTDlPJuhMd2iaSXcTXw1btVzADCuF+OA5FFHUnnNcOar1krYGVcAi6af0fUGZ6uGu1Z7WPQIDlFHMrWV7TqrQjkAJ5hF01abfCCXSw72jNYIViyu4xeAIOwPPwGd6LfVqzFtbOaOcIHytMh1oam7EPz7FHuPu1x7S/a0OERDbk0q4B2A2/pvhHaAwioBdvw07cjXsYF3Mv08dt46cNfUM45MAiGuVwBzxACPTDafgXfImfM1bWwnayL2hztH9DIlTSKfWThCBM46c0dtKZjqEJZ+FCrMbN+DDuwTeYXGYl42N+zNzNfMIuZdewG9k3uDu5GN/FP2JKHLqgHdNe1N6EaWCDW2EDbKHTnYIz8B/4ClmKNR0dWIxuXEsjgvuZfjyA/Uw1DuIZ5hC+jx/i53iR4ZkkZirjZDqZ3Uw3c4p5lW1h97CPsu+zF7gFPMMf4D82OczvDtUPbR96VSvWzmlfUD0KYKebccNSWAdBOm0H3AQ/oVMcpnGEbu00vAAvG+NDnA7n4QtCATAF03A2LqGxFJdhE7bg4zhA44SRy38ZuggmgUlmpjHTmVqmnmlnIsybTIRNZ3PZxexq9giNl9iz7EX2Isdz13JTuUVcBXRx7dw+Gk9xT3Mx7k98Eb+AX8qv4iP8dr6LbeBf48+atph2mmKmz03/MGebq8x3mLvodl6mmn0eRn84nEHZz4bboQE9WA976TYOYBCiVF2N+ADl2AHZWh27hV3EzKJqOAH3ULXug82wnV0DB7S32EPwZ6qUNooVgd9xbrDxv6DbuRdmURV9O3bTrT8Jz9B70U04ATiHVhrvnZ0/AVmunNyc7KxMxwz5erskZtimp6elWqddN3XKtSnJlslJiZMSBLOJ51gGIc8rlwUkJTOgcJlyeXm+LstBUgRHKQKKRKqysT6KFDDcpLGeLvJsuszTFfd0jXiiRZoP8/PzJK8sKa94ZEnF1ct9xD/okf2Sct7glxj8LoOfTLzdTgskr7XZIykYkLxKWbg56g14KFy/iyCYlJ+nf7G4IFEPrMDC4OZmK026h1dJkz1eJVX2GDbW4Q02KtXLfV5Put3uJx2pany0R35ei54n7EhqlBt3qC6oD+hccI1PYYN+hQnosZKdyjTZo0zb9LH1W/ES5+0aZVQYR1kwFC0jCHaUx8WALgW7SKqslSgss83vU3DbcBJ6jq2eeLoh2aurAq2SkiC75eZoa4DAhRpfLM2V5pWDHr8C1b5YqivVEPLz+q1biu10+v780vxSfS62W7fE50/vi+tfH0w0/E5/QHNlzQgAqO8kV1CeitRgbCJTsoX6I1QI0YZCcqOPH+mYLZTPQoWhmmEdCu+oCCqR2ktpNHviyQVaPbGE1DT9DAG3n/wDUcs82ob8LbIUvQB0hfL5z8ZqgsMak8NyAXRWv+iRWiH7JT5sAKNvZ5Wb9fsNe4dl2eodpSBZh0bPWZmizK6s9tkVyU8KFZx5lfQTV+3rQdzpV1HbpoLH1k+/5Oy6tWTO00utxUP7k5CfR4pcO3E35EllFLhMrxUpKkUrGqNSmdRMxcQ5jJkMoah/JiFY6yOcYAXt6PKnj7Ahv38exZmpx+GMOFE/RWgdjtBqRKAA35DTrLxKOmZmtW+5T4l40hWXx0+3QOU7WO1TBuni/H7yKhjJlObNLdbhnGdTzgW5xNwYj1JLMSiEPxqNS7JdGYxG06P6OxaXVYTLFa5hBf1BoAcgRFWMVBumiGxPNzC3y3ZKy69jehOV9KWKUmHOlRGeOxrhmynbuQbChVcJ4aKJIDxvQggXj4/wfMq5WEf4lu8P4QVjEC65MsKu0QiXUrYuA2H3VUJ44UQQ9kwIYe/4CJdRzl4d4UXfH8LlYxCuuDLCi0cjXEnZLjYQrrpKCC+ZCMJLJ4TwsvERrqacl+kIL//+EK4Zg3DtlRFeMRrhlZTtCgPhVVcJ4R9OBGHfhBD2j4/wasrZryN86wjCrnQFRiMcuQxQuOqQrxkDed2VIV87GvJ1lP5aA/LAVYI8OBHI6ycEecP4kDdSzg065KH/I+RNoyAHjDcHv3T0FK27Zv4FSBYMed2SnxnzXz644ewXoa+zEh8SvjT+m4DDK+hpyhnKoVYfyX4+8aFLkUY+DJ8CbqZoRG4zSPdiqKdKgNuog2fAQmM9gPlvibuol0YqAScOAI/9sM6JJ/
+EYLKDmK4fajBRaGHKexN9TYzZWcxzmjdHASXwOlsAtcDP1t5ecqEpgmaFJH9b0Uy97y5hAA5eFBmreKKlGp4pH47cY/zdFBVEJ0Rwip7PUChF8CnYRPUnEQgvugI1E24keJeJGuINE/bgjxgmuAdwIabjYlciJK6akitZJieLrKpr6Hhfftn54DFNhMpzD1NhkSCidhE/iE9AIIv4WHLiJGvBs3Neb0yYGyHQQOogiRKzxRDwYy5gtnsA8cHBIazIhg8Oj4qcF+eLHBSqDMfFUlsrR9HwGSa5rxEHb4+JJ23rxBFF33HQoR9XXHLS1ibszVNwXE39uU5EMD8Wnu2y09KjYnrNXbCww7FV7VaY7JhaRfZUrUZxbaBfn2D4SZ2apApKcb6sScwteEWfYDDeJgjpcyeJ0225xHpkybN6seUTH8BDuh1zcH3MsFgeIpeP2VuQU7lXxnt7y7AKHiptcc8uz9+aUZzlyqkRHTllWFvGrXjJvNd9qLjXPNjupB840283p5ilCimARfiAkCZMEQTCr+EysRDQdw24oIVi6ewWTwKv4LCm5Y3jYUB5+TuAERgBhiqp90KcX+RQVu/ssOkfMUZPBmVQ83BtXHXaJnM5xhsHC6E8m/nYwKDCwmFqHB1UTbLsuXGItSVmQXFTm+a5HYMzT+d0fK9qUvfQKK4dsfuociNFs/hHjFRbGP5130SPkdjorazb2hjtam4xOSPaGiALKjjB1ppF6Sepp7Rhu8zID9Q3N+hwMKR1yyKO0yh6pJ9w0jrlJN4dlTw80eVf4eppcIU8s7AobTWBvvXtD3Zi9to/stcE9TjC3HmyDvld93TjmOt1cr+9Vp+9Vp+9V76o39tLP6W2pdd/ZSdVJX8T0ZZtdq1QsX+1TpKDfo+JT+rfzXQD/A86W338KZW5kc3RyZWFtCmVuZG9iagoxOCAwIG9iagogICAyNzI4CmVuZG9iagoxOSAwIG9iago8PCAvTGVuZ3RoIDIwIDAgUgogICAvRmlsdGVyIC9GbGF0ZURlY29kZQo+PgpzdHJlYW0KeJxdkMFqwzAMhu9+Ch3bQ3HTWyEERnfJYetY2gdwbDkzLLJRnEPevoobOpjAFpL+z/yWvrTvLYUM+ouj7TCDD+QYpzizRehxCKSqE7hg81aV244mKS1wt0wZx5Z8VHUN+luGU+YFdm8u9rhXAKCv7JADDbC7X7pnq5tT+sURKcNRNQ049PLch0mfZkTQBT60TuYhLwfB/hS3JSGcSl09LdnocErGIhsaUNVHiQZqL9EoJPdvvlG9tz+Gi7oStaRzUW/9lVs/+TJlZ2bxUzZRjKwWAuFrWSmmlSrnATZrcGgKZW5kc3RyZWFtCmVuZG9iagoyMCAwIG9iagogICAyMjQKZW5kb2JqCjIxIDAgb2JqCjw8IC9UeXBlIC9Gb250RGVzY3JpcHRvcgogICAvRm9udE5hbWUgL1FWS0xKWitIZWx2ZXRpY2EKICAgL0ZvbnRGYW1pbHkgKEhlbHZldGljYSkKICAgL0ZsYWdzIDQKICAgL0ZvbnRCQm94IFsgLTk1MCAtNDgwIDE0NDUgMTEyMSBdCiAgIC9JdGFsaWNBbmdsZSAwCiAgIC9Bc2NlbnQgNzcwCiAgIC9EZXNjZW50IC0yMjkKICAgL0NhcEhlaWdodCAxMTIxCiAgIC9TdGVtViA4MAogICAvU3RlbUggODAKICAgL0ZvbnRGaWxlMiAxNyAwIFIKPj4KZW5kb2JqCjIyIDAgb2JqCjw8IC9UeXBlIC9Gb250CiAgIC9TdWJ0eXBlIC9DSURGb250VHlwZTIKICAgL0Jhc2VGb250IC9RVktMSlorSGVsdmV0aWNhCiAgIC9DSURTeXN0ZW1JbmZvCiAgIDw8IC9SZWdpc3RyeSAoQWRvYmUpCiAgICAgIC9PcmRlcmluZyAoSWRlbnRpdHkpCiAgICAgIC9TdXBwbGVtZW50IDAKICAgPj4KICAgL0ZvbnREZXNjcmlwdG9yIDIxIDAgUgogICAvVyBbMCBbIDYzMy43ODkwNjIgMjc3LjgzMjAzMSBdXQo+PgplbmRvYmoKOCAwIG9iago8PCAvVHlwZSAvRm9udAogICAvU3VidHlwZSAvVHlwZTAKICAgL0Jhc2VGb250IC9RVktMSlorSGVsdmV0aWNhCiAgIC9FbmNvZGluZyAvSWRlbnRpdHktSAogICAvRGVzY2VuZGFudEZvbnRzIFsgMjIgMCBSXQogICAvVG9Vbmljb2RlIDE5IDAgUgo+PgplbmRvYmoKMTEgMCBvYmoKPDwgL1R5cGUgL09ialN0bQogICAvTGVuZ3RoIDI1IDAgUgogICAvTiA0CiAgIC9GaXJzdCAyMwogICAvRmlsdGVyIC9GbGF0ZURlY29kZQo+PgpzdHJlYW0KeJxVkdFqwjAUhu/7FOdmTBmkSZpoleKFCiJjILq7uYsQQy0bTUnSMd9+J7XtNgKB8yVfzvkJA5rwDCTuwKlMuAAheFIUkL7eGgPpQZXGJwCQPlcXD2/AgcIR3ju0sW0dgCWrVWccnL202jiYaFU5C4ywnFCYXENo/DJNO1o61Vwr7Yl15XR6f8YZFSxq+/rDa4VtGckIh/NoVv1BlM5/rcrWWxUMTLZLTrmkGZ/xjIls/kTZI6XTYbTfMPCAA0f/oJyJ08c8HXgxl0qt7TeGpLjkQhI+l3LBIBeM5PliPhNj8Dqg7EGM9s7ZtoGiiEWs7x07OqATUqdq38TO+jbgPQTXmqHa4K2t+aq0Oe7WEWKCyI/G29Zp4yEbe55Q1OEexONP/gu7UUF92rLPir/YR8VLP5YSgooKZW5kc3RyZWFtCmVuZG9iagoyNSAwIG9iagogICAzMTEKZW5kb2JqCjI2IDAgb2JqCjw8IC9UeXBlIC9YUmVmCiAgIC9MZW5ndGggMTA0CiAgIC9GaWx0ZXIgL0ZsYXRlRGVjb2RlCiAgIC9TaXplIDI3CiAgIC9XIFsxIDIgMl0KICAgL1Jvb3QgMjQgMCBSCiAgIC9JbmZvIDIzIDAgUgo+PgpzdHJlYW0KeJxjYGD4/5+JgZuBAUQwMTLGMDAwMvADCUY3kBgnkKUKlGU0fQQSuwMkmOKBhFkjiFUKJJQkQIQBkFB+ASL+Awn1SiBhBFJiNBNIGJ8AEfeBhMkriEWMIIKZ0UIXKGbhwsAAAAHyD6IKZW5kc3RyZWFtCmVuZG9iagpzdGFydHhyZWYKMTQ0MDQKJSVFT0YK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extra-report.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra Report</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://ror.org/02w65pw28</t>
   </si>
   <si>
@@ -1247,7 +1295,7 @@
     <t xml:space="preserve"> Master</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes</t>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">second cycle</t>
@@ -1319,9 +1367,15 @@
     <t xml:space="preserve">Music study programme group</t>
   </si>
   <si>
+    <t xml:space="preserve">Muusika õppeprogrammi rühm</t>
+  </si>
+  <si>
     <t xml:space="preserve">magistriõppe</t>
   </si>
   <si>
+    <t xml:space="preserve">full degree</t>
+  </si>
+  <si>
     <t xml:space="preserve">MusiQuE20</t>
   </si>
   <si>
@@ -1409,9 +1463,6 @@
     <t xml:space="preserve">CoPeCo  is  a  joint  study  programme,  i.e. a programme to be carried out jointly by several institutions in different countries, and which does not lead to a joint degree. Quality enhancement review of the Contemporay Performance and Composition joint programme coordinated by the Estonian Academy of Music and Theater.</t>
   </si>
   <si>
-    <t xml:space="preserve">link_display_name[2]</t>
-  </si>
-  <si>
     <t xml:space="preserve">ZEvA</t>
   </si>
   <si>
@@ -1427,6 +1478,9 @@
     <t xml:space="preserve">de</t>
   </si>
   <si>
+    <t xml:space="preserve">DEQARINST0002</t>
+  </si>
+  <si>
     <t xml:space="preserve">DEQARINST8785</t>
   </si>
   <si>
@@ -1454,7 +1508,7 @@
     <t xml:space="preserve">31/08/2023</t>
   </si>
   <si>
-    <t xml:space="preserve">d%/%m/%Y</t>
+    <t xml:space="preserve">%d/%m/%Y</t>
   </si>
   <si>
     <t xml:space="preserve">https://iaar.agency/storage/photos/shares/inst_accreditation_files/Zerde_310823/Rewenie.pdf</t>
@@ -1473,6 +1527,9 @@
   </si>
   <si>
     <t xml:space="preserve">RU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEQARINST8612</t>
   </si>
 </sst>
 </file>
@@ -2057,10 +2114,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AQ2"/>
+  <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2080,31 +2137,32 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="21.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="16.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="16.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="24.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="26.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="31" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="26.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="22.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="20.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="24.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="21.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="14.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="19.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="21.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="17.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="16.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="16.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="24.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="26.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="32" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="26.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="22.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="22.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="24.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="21.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="14.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="16.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2159,16 +2217,16 @@
       <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="8" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="5" t="s">
@@ -2177,7 +2235,7 @@
       <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
       <c r="Y1" s="9" t="s">
@@ -2192,7 +2250,7 @@
       <c r="AB1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="9" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="6" t="s">
@@ -2201,7 +2259,7 @@
       <c r="AE1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" s="6" t="s">
         <v>31</v>
       </c>
       <c r="AG1" s="7" t="s">
@@ -2210,16 +2268,16 @@
       <c r="AH1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="10" t="s">
+      <c r="AK1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AL1" s="10" t="s">
         <v>37</v>
       </c>
       <c r="AM1" s="11" t="s">
@@ -2234,133 +2292,137 @@
       <c r="AP1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="9" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>42</v>
+      </c>
+      <c r="AR1" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="E2" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="J2" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="M2" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="S2" s="13" t="s">
+      <c r="U2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="AF2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="AK2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="13" t="s">
+      <c r="AL2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL2" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="AM2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN2" s="13" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="AN2" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="AO2" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AP2" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AQ2" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="AR2" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2378,10 +2440,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2395,16 +2457,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="23" style="0" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="21.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="20.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="41.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="15.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="15.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="25" style="0" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="21.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="20.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="41.52"/>
   </cols>
   <sheetData>
     <row r="1" s="20" customFormat="true" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2483,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>8</v>
@@ -2442,69 +2504,75 @@
         <v>14</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="X1" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Y1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z1" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>22</v>
+        <v>60</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA1" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="AB1" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="19" t="s">
-        <v>42</v>
+      <c r="AD1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="101.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D2" s="22" t="n">
         <v>183</v>
@@ -2513,10 +2581,10 @@
         <v>543</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H2" s="24" t="n">
         <v>43546</v>
@@ -2525,73 +2593,75 @@
         <v>45747</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N2" s="23" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="O2" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="P2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="S2" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="T2" s="23" t="s">
+      <c r="U2" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="23" t="s">
         <v>73</v>
-      </c>
-      <c r="U2" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="W2" s="23" t="s">
-        <v>74</v>
       </c>
       <c r="X2" s="23" t="s">
         <v>75</v>
       </c>
       <c r="Y2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z2" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="21" t="s">
         <v>77</v>
       </c>
+      <c r="Z2" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA2" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB2" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC2" s="22"/>
       <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
+      <c r="AE2" s="21" t="s">
+        <v>80</v>
+      </c>
       <c r="AF2" s="22"/>
       <c r="AG2" s="22"/>
+      <c r="AH2" s="22"/>
+      <c r="AI2" s="22"/>
     </row>
-    <row r="3" customFormat="false" ht="90.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="103.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D3" s="22" t="n">
         <v>97</v>
@@ -2608,47 +2678,57 @@
       </c>
       <c r="I3" s="24"/>
       <c r="J3" s="23" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="O3" s="23" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="P3" s="23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
+      <c r="R3" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="S3" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="T3" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="U3" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
       <c r="X3" s="21"/>
-      <c r="Y3" s="22"/>
+      <c r="Y3" s="21"/>
       <c r="Z3" s="21"/>
-      <c r="AA3" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB3" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC3" s="22"/>
-      <c r="AD3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD3" s="22" t="s">
+        <v>90</v>
+      </c>
       <c r="AE3" s="22"/>
       <c r="AF3" s="22"/>
       <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2726,191 +2806,191 @@
         <v>14</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="R1" s="19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X1" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y1" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z1" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA1" s="18" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="AB1" s="18" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="AC1" s="18" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="AD1" s="18" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="AE1" s="18" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="AF1" s="18" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="AG1" s="18" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="AH1" s="18" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="AI1" s="18" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="AJ1" s="18" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="AK1" s="18" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="AL1" s="18" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="AM1" s="18" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="AN1" s="18" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="AO1" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="79.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C2" s="22" t="n">
         <v>181</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F2" s="24" t="n">
         <v>43538</v>
       </c>
       <c r="G2" s="24"/>
       <c r="H2" s="23" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="N2" s="23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O2" s="22"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
       <c r="R2" s="21" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="S2" s="25"/>
       <c r="T2" s="26" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="U2" s="21" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="V2" s="27" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="W2" s="27"/>
       <c r="X2" s="27"/>
       <c r="Y2" s="27" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="Z2" s="27" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="AA2" s="26" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="AB2" s="23" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="AC2" s="23" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="AD2" s="22"/>
       <c r="AE2" s="27"/>
       <c r="AF2" s="21" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="AG2" s="21" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="101.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C3" s="22" t="n">
         <v>184</v>
@@ -2928,47 +3008,47 @@
         <v>45473</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O3" s="22"/>
       <c r="P3" s="22"/>
       <c r="Q3" s="22"/>
       <c r="R3" s="21" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="S3" s="22"/>
       <c r="T3" s="26" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="U3" s="21" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="V3" s="23" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="W3" s="21" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="X3" s="21" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="Y3" s="0" t="n">
         <v>1</v>
@@ -2977,19 +3057,19 @@
         <v>2</v>
       </c>
       <c r="AA3" s="26" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="AB3" s="21" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="AC3" s="23" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="AD3" s="21" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="AE3" s="21" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="AF3" s="26" t="n">
         <v>1</v>
@@ -2998,19 +3078,19 @@
         <v>1</v>
       </c>
       <c r="AH3" s="26" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="AI3" s="21" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="AJ3" s="21" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="AK3" s="21" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="AL3" s="21" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="AM3" s="25" t="n">
         <v>1</v>
@@ -3021,10 +3101,10 @@
     </row>
     <row r="4" customFormat="false" ht="79.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C4" s="25" t="n">
         <v>181</v>
@@ -3040,16 +3120,16 @@
       </c>
       <c r="G4" s="25"/>
       <c r="H4" s="23" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L4" s="25"/>
       <c r="M4" s="25"/>
@@ -3059,42 +3139,46 @@
       <c r="Q4" s="25"/>
       <c r="R4" s="25"/>
       <c r="S4" s="29" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="T4" s="26" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="U4" s="29" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="V4" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="W4" s="21"/>
+        <v>124</v>
+      </c>
+      <c r="W4" s="21" t="s">
+        <v>137</v>
+      </c>
       <c r="X4" s="29" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="Y4" s="0" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="Z4" s="22" t="n">
         <v>2</v>
       </c>
       <c r="AA4" s="26" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="AB4" s="29" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="AC4" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD4" s="21"/>
+        <v>116</v>
+      </c>
+      <c r="AD4" s="21" t="s">
+        <v>137</v>
+      </c>
       <c r="AE4" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF4" s="21" t="s">
-        <v>107</v>
+        <v>141</v>
+      </c>
+      <c r="AF4" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="AG4" s="25" t="n">
         <v>1</v>
@@ -3102,19 +3186,19 @@
     </row>
     <row r="5" customFormat="false" ht="113.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C5" s="29" t="n">
         <v>181</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F5" s="28" t="n">
         <v>43999</v>
@@ -3123,76 +3207,76 @@
         <v>46203</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="R5" s="25"/>
       <c r="S5" s="29" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="U5" s="21" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="V5" s="21" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="W5" s="29" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="X5" s="25"/>
       <c r="Y5" s="22" t="n">
         <v>1</v>
       </c>
       <c r="Z5" s="23" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="AA5" s="26" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="AB5" s="23" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="AC5" s="23" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="AD5" s="29" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="AE5" s="25"/>
       <c r="AF5" s="25" t="n">
         <v>1</v>
       </c>
       <c r="AG5" s="21" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="AH5" s="25"/>
       <c r="AI5" s="25"/>
@@ -3202,7 +3286,7 @@
       <c r="AM5" s="25"/>
       <c r="AN5" s="25"/>
       <c r="AO5" s="29" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3261,7 +3345,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>8</v>
@@ -3282,54 +3366,54 @@
         <v>14</v>
       </c>
       <c r="L1" s="33" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M1" s="33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="P1" s="34" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="R1" s="33" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S1" s="33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T1" s="33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U1" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="33" t="s">
-        <v>34</v>
-      </c>
       <c r="W1" s="33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X1" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="124.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="35" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="D2" s="36" t="n">
         <v>182</v>
@@ -3338,61 +3422,61 @@
         <v>499</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="H2" s="38" t="n">
-        <v>41654</v>
+        <v>45306</v>
       </c>
       <c r="I2" s="38" t="n">
-        <v>43130</v>
+        <v>46782</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K2" s="37" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="L2" s="35" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="M2" s="36" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="P2" s="37" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="Q2" s="35" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="R2" s="26" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="S2" s="37" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="T2" s="37" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="U2" s="37" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="V2" s="37" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="W2" s="37" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="X2" s="29" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3424,7 +3508,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3432,6 +3516,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="14.71"/>
@@ -3452,7 +3538,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>8</v>
@@ -3476,72 +3562,72 @@
         <v>14</v>
       </c>
       <c r="M1" s="33" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N1" s="41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O1" s="40" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P1" s="40" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="R1" s="33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="S1" s="41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="T1" s="33" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U1" s="33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V1" s="34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W1" s="34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X1" s="34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Y1" s="34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Z1" s="40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA1" s="42" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AB1" s="42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AC1" s="42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AD1" s="42" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AE1" s="42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AF1" s="42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="43" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>141</v>
@@ -3556,36 +3642,36 @@
         <v>42613</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="O2" s="45"/>
       <c r="P2" s="45"/>
       <c r="Q2" s="46"/>
       <c r="R2" s="46"/>
       <c r="S2" s="46"/>
-      <c r="T2" s="0" t="n">
-        <v>93962</v>
+      <c r="T2" s="0" t="s">
+        <v>174</v>
       </c>
       <c r="U2" s="29" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="W2" s="29" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="Y2" s="0" t="n">
         <v>3</v>
@@ -3600,13 +3686,13 @@
         <v>2</v>
       </c>
       <c r="AD2" s="45" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="AE2" s="45" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="AF2" s="47" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3614,7 +3700,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>22367</v>
@@ -3632,40 +3718,40 @@
         <v>1</v>
       </c>
       <c r="I3" s="49" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="J3" s="50" t="n">
         <v>46996</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>7788</v>
+        <v>190</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>